<commit_message>
add infinity pool function
</commit_message>
<xml_diff>
--- a/FGO/FGO.xlsx
+++ b/FGO/FGO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongl2/Desktop/personal/GitHub/auto_js_scripts/FGO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0159C82-8B38-8C45-85D6-C4453D9A4BBF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E194876-8CDC-D449-B3FE-CED790D7AF55}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="460" windowWidth="32740" windowHeight="20540" xr2:uid="{6A258196-762F-264E-80CE-4732B31805C7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t>KEY</t>
   </si>
@@ -320,9 +320,6 @@
   </si>
   <si>
     <t>关闭重置选项</t>
-  </si>
-  <si>
-    <t>0.5s</t>
   </si>
 </sst>
 </file>
@@ -625,15 +622,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -646,40 +673,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1096,9 +1093,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952D6C80-24B6-9C4C-A7F3-85A241643D50}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="162" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1114,18 +1111,18 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="8"/>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="51" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51" t="s">
+      <c r="E1" s="53"/>
+      <c r="F1" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="51"/>
+      <c r="G1" s="53"/>
       <c r="H1" s="39" t="s">
         <v>77</v>
       </c>
@@ -1202,10 +1199,10 @@
       <c r="H3" s="41">
         <v>1</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="54" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1237,8 +1234,8 @@
       <c r="H4" s="41">
         <v>1</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="9" t="s">
@@ -1268,8 +1265,8 @@
       <c r="H5" s="41">
         <v>1</v>
       </c>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="9" t="s">
@@ -1299,8 +1296,8 @@
       <c r="H6" s="41">
         <v>1</v>
       </c>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="9" t="s">
@@ -1330,8 +1327,8 @@
       <c r="H7" s="41">
         <v>1</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="9" t="s">
@@ -1361,8 +1358,8 @@
       <c r="H8" s="41">
         <v>1</v>
       </c>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="9" t="s">
@@ -1392,8 +1389,8 @@
       <c r="H9" s="41">
         <v>1</v>
       </c>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="9" t="s">
@@ -1423,8 +1420,8 @@
       <c r="H10" s="41">
         <v>1</v>
       </c>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="9" t="s">
@@ -1454,8 +1451,8 @@
       <c r="H11" s="41">
         <v>1</v>
       </c>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="10" t="s">
@@ -1485,10 +1482,10 @@
       <c r="H12" s="42">
         <v>0</v>
       </c>
-      <c r="I12" s="58" t="s">
+      <c r="I12" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="58" t="s">
+      <c r="J12" s="56" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1520,8 +1517,8 @@
       <c r="H13" s="42">
         <v>0</v>
       </c>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="10" t="s">
@@ -1551,8 +1548,8 @@
       <c r="H14" s="42">
         <v>0</v>
       </c>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="10" t="s">
@@ -1582,8 +1579,8 @@
       <c r="H15" s="42">
         <v>0</v>
       </c>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="10" t="s">
@@ -1613,8 +1610,8 @@
       <c r="H16" s="42">
         <v>0</v>
       </c>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="11" t="s">
@@ -1644,10 +1641,10 @@
       <c r="H17" s="43">
         <v>0</v>
       </c>
-      <c r="I17" s="60" t="s">
+      <c r="I17" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="60" t="s">
+      <c r="J17" s="58" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1679,8 +1676,8 @@
       <c r="H18" s="43">
         <v>0</v>
       </c>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="11" t="s">
@@ -1710,8 +1707,8 @@
       <c r="H19" s="43">
         <v>0</v>
       </c>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="12" t="s">
@@ -1776,10 +1773,10 @@
       <c r="H21" s="44">
         <v>1</v>
       </c>
-      <c r="I21" s="62" t="s">
+      <c r="I21" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="J21" s="62" t="s">
+      <c r="J21" s="66" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1811,8 +1808,8 @@
       <c r="H22" s="44">
         <v>1</v>
       </c>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="12" t="s">
@@ -1842,8 +1839,8 @@
       <c r="H23" s="44">
         <v>1</v>
       </c>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="13" t="s">
@@ -1873,10 +1870,10 @@
       <c r="H24" s="45">
         <v>0</v>
       </c>
-      <c r="I24" s="52" t="s">
+      <c r="I24" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="J24" s="52" t="s">
+      <c r="J24" s="62" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1908,8 +1905,8 @@
       <c r="H25" s="45">
         <v>0</v>
       </c>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="63"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="13" t="s">
@@ -1939,8 +1936,8 @@
       <c r="H26" s="45">
         <v>0</v>
       </c>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="14" t="s">
@@ -2005,10 +2002,10 @@
       <c r="H28" s="46">
         <v>0</v>
       </c>
-      <c r="I28" s="54" t="s">
+      <c r="I28" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="J28" s="54" t="s">
+      <c r="J28" s="64" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2040,8 +2037,8 @@
       <c r="H29" s="46">
         <v>0</v>
       </c>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="I29" s="65"/>
+      <c r="J29" s="65"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="14" t="s">
@@ -2071,8 +2068,8 @@
       <c r="H30" s="46">
         <v>0</v>
       </c>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="14" t="s">
@@ -2102,8 +2099,8 @@
       <c r="H31" s="46">
         <v>0</v>
       </c>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="14" t="s">
@@ -2133,8 +2130,8 @@
       <c r="H32" s="46">
         <v>0</v>
       </c>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="14" t="s">
@@ -2234,10 +2231,10 @@
       <c r="H35" s="47">
         <v>0</v>
       </c>
-      <c r="I35" s="49" t="s">
+      <c r="I35" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="J35" s="49" t="s">
+      <c r="J35" s="60" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2269,8 +2266,8 @@
       <c r="H36" s="47">
         <v>0</v>
       </c>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
+      <c r="I36" s="61"/>
+      <c r="J36" s="61"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="15" t="s">
@@ -2300,8 +2297,8 @@
       <c r="H37" s="47">
         <v>0</v>
       </c>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="61"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="15" t="s">
@@ -2331,8 +2328,8 @@
       <c r="H38" s="47">
         <v>0</v>
       </c>
-      <c r="I38" s="50"/>
-      <c r="J38" s="50"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="15" t="s">
@@ -2362,8 +2359,8 @@
       <c r="H39" s="47">
         <v>0</v>
       </c>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="61"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="15" t="s">
@@ -2393,8 +2390,8 @@
       <c r="H40" s="47">
         <v>0</v>
       </c>
-      <c r="I40" s="50"/>
-      <c r="J40" s="50"/>
+      <c r="I40" s="61"/>
+      <c r="J40" s="61"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="18" t="s">
@@ -2512,11 +2509,11 @@
         <v>647</v>
       </c>
       <c r="D44" s="19">
-        <f t="shared" ref="D44" si="6">B44</f>
+        <f t="shared" ref="D44:D47" si="6">B44</f>
         <v>584</v>
       </c>
       <c r="E44" s="19">
-        <f t="shared" ref="E44" si="7">C44</f>
+        <f t="shared" ref="E44:E47" si="7">C44</f>
         <v>647</v>
       </c>
       <c r="F44" s="33">
@@ -2540,16 +2537,26 @@
       <c r="A45" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
+      <c r="B45" s="19">
+        <v>1710</v>
+      </c>
+      <c r="C45" s="19">
+        <v>365</v>
+      </c>
+      <c r="D45" s="19">
+        <f t="shared" si="6"/>
+        <v>1710</v>
+      </c>
+      <c r="E45" s="19">
+        <f t="shared" si="7"/>
+        <v>365</v>
+      </c>
       <c r="F45" s="33">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="G45" s="24">
         <f t="shared" ref="G45:G47" si="9">F45/1000</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="H45" s="42">
         <v>0</v>
@@ -2557,24 +2564,34 @@
       <c r="I45" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="J45" s="65" t="s">
-        <v>89</v>
+      <c r="J45" s="49" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
+      <c r="B46" s="19">
+        <v>1255</v>
+      </c>
+      <c r="C46" s="19">
+        <v>840</v>
+      </c>
+      <c r="D46" s="19">
+        <f t="shared" si="6"/>
+        <v>1255</v>
+      </c>
+      <c r="E46" s="19">
+        <f t="shared" si="7"/>
+        <v>840</v>
+      </c>
       <c r="F46" s="33">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="G46" s="24">
         <f t="shared" si="9"/>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="H46" s="42">
         <v>0</v>
@@ -2582,22 +2599,32 @@
       <c r="I46" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="J46" s="66"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
+      <c r="B47" s="19">
+        <v>960</v>
+      </c>
+      <c r="C47" s="19">
+        <v>840</v>
+      </c>
+      <c r="D47" s="19">
+        <f t="shared" si="6"/>
+        <v>960</v>
+      </c>
+      <c r="E47" s="19">
+        <f t="shared" si="7"/>
+        <v>840</v>
+      </c>
       <c r="F47" s="33">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="G47" s="24">
         <f t="shared" si="9"/>
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="H47" s="42">
         <v>0</v>
@@ -2605,10 +2632,12 @@
       <c r="I47" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="J47" s="67"/>
+      <c r="J47" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="J28:J32"/>
+    <mergeCell ref="I21:I23"/>
     <mergeCell ref="J45:J47"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
@@ -2625,8 +2654,6 @@
     <mergeCell ref="J17:J19"/>
     <mergeCell ref="J21:J23"/>
     <mergeCell ref="J24:J26"/>
-    <mergeCell ref="J28:J32"/>
-    <mergeCell ref="I21:I23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add yanzuo_xiaomo_auto for using in the night
</commit_message>
<xml_diff>
--- a/FGO/FGO.xlsx
+++ b/FGO/FGO.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongl2/Desktop/personal/GitHub/auto_js_scripts/FGO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\auto_js_scripts\FGO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E194876-8CDC-D449-B3FE-CED790D7AF55}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="32740" windowHeight="20540" xr2:uid="{6A258196-762F-264E-80CE-4732B31805C7}"/>
+    <workbookView xWindow="855" yWindow="465" windowWidth="32745" windowHeight="20535"/>
   </bookViews>
   <sheets>
     <sheet name="Pexel LUT" sheetId="1" r:id="rId1"/>
     <sheet name="Measured" sheetId="2" r:id="rId2"/>
     <sheet name="Actual" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="132">
   <si>
     <t>KEY</t>
   </si>
@@ -321,19 +319,225 @@
   <si>
     <t>关闭重置选项</t>
   </si>
+  <si>
+    <t>0.5s</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTASK</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择default置顶任务</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_AP50</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHIJIE0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHIJIE1</t>
+  </si>
+  <si>
+    <t>ZHIJIE2</t>
+  </si>
+  <si>
+    <t>ZHIJIE3</t>
+  </si>
+  <si>
+    <t>ZHIJIE4</t>
+  </si>
+  <si>
+    <t>ZHIJIE5</t>
+  </si>
+  <si>
+    <t>ZHIJIE6</t>
+  </si>
+  <si>
+    <t>ZHIJIE7</t>
+  </si>
+  <si>
+    <t>ZHIJIE8</t>
+  </si>
+  <si>
+    <t>选择助战-职介-0-全</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择助战-职介-1-剑</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择助战-职介-2-弓</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择助战-职介-3-枪</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择助战-职介-4-骑</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择助战-职介-5-术</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择助战-职介-6-杀</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择助战-职介-7-狂</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择助战-职介-8-外</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳过剧情-是</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳过剧情-否</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKIPY</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKIPN</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKIPS</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳过剧情-选择</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>DZHUZHAN</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择助战好友-default第一个</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1s</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2s</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">30s  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>加载战斗</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>AP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>约等于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Songti SC Regular"/>
+      </rPr>
+      <t>45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的位置点</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加体力</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>AuAPPLE</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDAP</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONFIRM</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CANCLE</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>金苹果</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>确认</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKIPP/N</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="00000"/>
+    <numFmt numFmtId="176" formatCode="00000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -341,7 +545,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -371,6 +575,25 @@
       <b/>
       <sz val="12"/>
       <color theme="9"/>
+      <name val="Songti SC Regular"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Songti SC Regular"/>
     </font>
   </fonts>
@@ -488,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -622,6 +845,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -631,7 +869,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -667,21 +905,18 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -716,7 +951,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6B4FA6B-D066-4644-8083-E69566C80E15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6B4FA6B-D066-4644-8083-E69566C80E15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -765,7 +1000,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E186714-FDDD-E74D-B31E-D615057E762A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2E186714-FDDD-E74D-B31E-D615057E762A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1090,39 +1325,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952D6C80-24B6-9C4C-A7F3-85A241643D50}">
-  <dimension ref="A1:L47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67:XFD79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="10.83203125" style="7"/>
-    <col min="6" max="6" width="13.83203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.625" style="7" customWidth="1"/>
+    <col min="2" max="5" width="10.875" style="7"/>
+    <col min="6" max="6" width="13.875" style="7" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="22" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="48" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" style="16" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="5"/>
+    <col min="9" max="9" width="31.375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="24.625" style="16" customWidth="1"/>
+    <col min="11" max="16384" width="10.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="8"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="53" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53" t="s">
+      <c r="E1" s="58"/>
+      <c r="F1" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="53"/>
+      <c r="G1" s="58"/>
       <c r="H1" s="39" t="s">
         <v>77</v>
       </c>
@@ -1136,7 +1372,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1407,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
@@ -1199,14 +1435,14 @@
       <c r="H3" s="41">
         <v>1</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -1234,10 +1470,10 @@
       <c r="H4" s="41">
         <v>1</v>
       </c>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
@@ -1265,10 +1501,10 @@
       <c r="H5" s="41">
         <v>1</v>
       </c>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -1296,10 +1532,10 @@
       <c r="H6" s="41">
         <v>1</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -1327,10 +1563,10 @@
       <c r="H7" s="41">
         <v>1</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
@@ -1358,10 +1594,10 @@
       <c r="H8" s="41">
         <v>1</v>
       </c>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
@@ -1389,10 +1625,10 @@
       <c r="H9" s="41">
         <v>1</v>
       </c>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1420,10 +1656,10 @@
       <c r="H10" s="41">
         <v>1</v>
       </c>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
@@ -1451,10 +1687,10 @@
       <c r="H11" s="41">
         <v>1</v>
       </c>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
@@ -1473,23 +1709,23 @@
         <v>800</v>
       </c>
       <c r="F12" s="33">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G12" s="24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H12" s="42">
         <v>0</v>
       </c>
-      <c r="I12" s="56" t="s">
+      <c r="I12" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="56" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="J12" s="61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1508,19 +1744,19 @@
         <v>800</v>
       </c>
       <c r="F13" s="33">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G13" s="24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H13" s="42">
         <v>0</v>
       </c>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
@@ -1539,19 +1775,19 @@
         <v>800</v>
       </c>
       <c r="F14" s="33">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G14" s="24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H14" s="42">
         <v>0</v>
       </c>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="10" t="s">
         <v>20</v>
       </c>
@@ -1570,19 +1806,19 @@
         <v>800</v>
       </c>
       <c r="F15" s="33">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G15" s="24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H15" s="42">
         <v>0</v>
       </c>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="10" t="s">
         <v>21</v>
       </c>
@@ -1601,19 +1837,19 @@
         <v>800</v>
       </c>
       <c r="F16" s="33">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G16" s="24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H16" s="42">
         <v>0</v>
       </c>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75">
       <c r="A17" s="11" t="s">
         <v>22</v>
       </c>
@@ -1641,14 +1877,14 @@
       <c r="H17" s="43">
         <v>0</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="58" t="s">
+      <c r="J17" s="63" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" ht="15.75">
       <c r="A18" s="11" t="s">
         <v>23</v>
       </c>
@@ -1676,10 +1912,10 @@
       <c r="H18" s="43">
         <v>0</v>
       </c>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75">
       <c r="A19" s="11" t="s">
         <v>24</v>
       </c>
@@ -1707,10 +1943,10 @@
       <c r="H19" s="43">
         <v>0</v>
       </c>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75">
       <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
@@ -1745,7 +1981,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" ht="15.75">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -1773,14 +2009,14 @@
       <c r="H21" s="44">
         <v>1</v>
       </c>
-      <c r="I21" s="66" t="s">
+      <c r="I21" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="J21" s="66" t="s">
+      <c r="J21" s="52" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" ht="15.75">
       <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
@@ -1808,10 +2044,10 @@
       <c r="H22" s="44">
         <v>1</v>
       </c>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75">
       <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
@@ -1839,10 +2075,10 @@
       <c r="H23" s="44">
         <v>1</v>
       </c>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75">
       <c r="A24" s="13" t="s">
         <v>29</v>
       </c>
@@ -1870,14 +2106,14 @@
       <c r="H24" s="45">
         <v>0</v>
       </c>
-      <c r="I24" s="62" t="s">
+      <c r="I24" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="J24" s="62" t="s">
+      <c r="J24" s="67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" ht="15.75">
       <c r="A25" s="13" t="s">
         <v>30</v>
       </c>
@@ -1905,10 +2141,10 @@
       <c r="H25" s="45">
         <v>0</v>
       </c>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
@@ -1936,10 +2172,10 @@
       <c r="H26" s="45">
         <v>0</v>
       </c>
-      <c r="I26" s="63"/>
-      <c r="J26" s="63"/>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75">
       <c r="A27" s="14" t="s">
         <v>34</v>
       </c>
@@ -1974,7 +2210,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" ht="15.75">
       <c r="A28" s="14" t="s">
         <v>56</v>
       </c>
@@ -2002,14 +2238,14 @@
       <c r="H28" s="46">
         <v>0</v>
       </c>
-      <c r="I28" s="64" t="s">
+      <c r="I28" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="J28" s="64" t="s">
+      <c r="J28" s="50" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" ht="15.75">
       <c r="A29" s="14" t="s">
         <v>57</v>
       </c>
@@ -2037,10 +2273,10 @@
       <c r="H29" s="46">
         <v>0</v>
       </c>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75">
       <c r="A30" s="14" t="s">
         <v>58</v>
       </c>
@@ -2068,10 +2304,10 @@
       <c r="H30" s="46">
         <v>0</v>
       </c>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75">
       <c r="A31" s="14" t="s">
         <v>59</v>
       </c>
@@ -2099,10 +2335,10 @@
       <c r="H31" s="46">
         <v>0</v>
       </c>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75">
       <c r="A32" s="14" t="s">
         <v>60</v>
       </c>
@@ -2130,10 +2366,10 @@
       <c r="H32" s="46">
         <v>0</v>
       </c>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75">
       <c r="A33" s="14" t="s">
         <v>61</v>
       </c>
@@ -2168,7 +2404,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="20">
+    <row r="34" spans="1:10" ht="15.75">
       <c r="A34" s="15" t="s">
         <v>41</v>
       </c>
@@ -2203,7 +2439,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" ht="15.75">
       <c r="A35" s="15" t="s">
         <v>35</v>
       </c>
@@ -2231,14 +2467,14 @@
       <c r="H35" s="47">
         <v>0</v>
       </c>
-      <c r="I35" s="60" t="s">
+      <c r="I35" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="J35" s="60" t="s">
+      <c r="J35" s="65" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" ht="15.75">
       <c r="A36" s="15" t="s">
         <v>36</v>
       </c>
@@ -2266,10 +2502,10 @@
       <c r="H36" s="47">
         <v>0</v>
       </c>
-      <c r="I36" s="61"/>
-      <c r="J36" s="61"/>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="I36" s="66"/>
+      <c r="J36" s="66"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75">
       <c r="A37" s="15" t="s">
         <v>37</v>
       </c>
@@ -2297,10 +2533,10 @@
       <c r="H37" s="47">
         <v>0</v>
       </c>
-      <c r="I37" s="61"/>
-      <c r="J37" s="61"/>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="I37" s="66"/>
+      <c r="J37" s="66"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.75">
       <c r="A38" s="15" t="s">
         <v>38</v>
       </c>
@@ -2328,10 +2564,10 @@
       <c r="H38" s="47">
         <v>0</v>
       </c>
-      <c r="I38" s="61"/>
-      <c r="J38" s="61"/>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="I38" s="66"/>
+      <c r="J38" s="66"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75">
       <c r="A39" s="15" t="s">
         <v>39</v>
       </c>
@@ -2359,10 +2595,10 @@
       <c r="H39" s="47">
         <v>0</v>
       </c>
-      <c r="I39" s="61"/>
-      <c r="J39" s="61"/>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="I39" s="66"/>
+      <c r="J39" s="66"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.75">
       <c r="A40" s="15" t="s">
         <v>40</v>
       </c>
@@ -2390,10 +2626,10 @@
       <c r="H40" s="47">
         <v>0</v>
       </c>
-      <c r="I40" s="61"/>
-      <c r="J40" s="61"/>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="I40" s="66"/>
+      <c r="J40" s="66"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75">
       <c r="A41" s="18" t="s">
         <v>43</v>
       </c>
@@ -2428,7 +2664,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" ht="15.75">
       <c r="A42" s="18" t="s">
         <v>53</v>
       </c>
@@ -2463,7 +2699,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" ht="15.75">
       <c r="A43" s="18" t="s">
         <v>78</v>
       </c>
@@ -2498,7 +2734,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" ht="15.75">
       <c r="A44" s="19" t="s">
         <v>81</v>
       </c>
@@ -2509,11 +2745,11 @@
         <v>647</v>
       </c>
       <c r="D44" s="19">
-        <f t="shared" ref="D44:D47" si="6">B44</f>
+        <f t="shared" ref="D44:D60" si="6">B44</f>
         <v>584</v>
       </c>
       <c r="E44" s="19">
-        <f t="shared" ref="E44:E47" si="7">C44</f>
+        <f t="shared" ref="E44:E60" si="7">C44</f>
         <v>647</v>
       </c>
       <c r="F44" s="33">
@@ -2533,7 +2769,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" ht="15.75">
       <c r="A45" s="19" t="s">
         <v>82</v>
       </c>
@@ -2555,7 +2791,7 @@
         <v>1500</v>
       </c>
       <c r="G45" s="24">
-        <f t="shared" ref="G45:G47" si="9">F45/1000</f>
+        <f t="shared" ref="G45:G60" si="9">F45/1000</f>
         <v>1.5</v>
       </c>
       <c r="H45" s="42">
@@ -2564,11 +2800,11 @@
       <c r="I45" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="J45" s="49" t="s">
+      <c r="J45" s="54" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" ht="15.75">
       <c r="A46" s="19" t="s">
         <v>85</v>
       </c>
@@ -2599,9 +2835,9 @@
       <c r="I46" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="J46" s="50"/>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="J46" s="55"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75">
       <c r="A47" s="19" t="s">
         <v>86</v>
       </c>
@@ -2632,10 +2868,649 @@
       <c r="I47" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="J47" s="51"/>
+      <c r="J47" s="56"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75">
+      <c r="A48" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="49">
+        <v>1050</v>
+      </c>
+      <c r="C48" s="49">
+        <v>345</v>
+      </c>
+      <c r="D48" s="49">
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="E48" s="49">
+        <f t="shared" si="7"/>
+        <v>345</v>
+      </c>
+      <c r="F48" s="32">
+        <v>3000</v>
+      </c>
+      <c r="G48" s="23">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="H48" s="41">
+        <v>0</v>
+      </c>
+      <c r="I48" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="J48" s="49"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75">
+      <c r="A49" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" s="49">
+        <v>240</v>
+      </c>
+      <c r="C49" s="49">
+        <v>465</v>
+      </c>
+      <c r="D49" s="49">
+        <f t="shared" ref="D49" si="10">B49</f>
+        <v>240</v>
+      </c>
+      <c r="E49" s="49">
+        <f t="shared" ref="E49" si="11">C49</f>
+        <v>465</v>
+      </c>
+      <c r="F49" s="32">
+        <v>3000</v>
+      </c>
+      <c r="G49" s="23">
+        <f t="shared" ref="G49" si="12">F49/1000</f>
+        <v>3</v>
+      </c>
+      <c r="H49" s="41">
+        <v>0</v>
+      </c>
+      <c r="I49" s="69" t="s">
+        <v>118</v>
+      </c>
+      <c r="J49" s="49"/>
+    </row>
+    <row r="50" spans="1:10" ht="15.75">
+      <c r="A50" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="49">
+        <v>335</v>
+      </c>
+      <c r="C50" s="49">
+        <v>1040</v>
+      </c>
+      <c r="D50" s="49">
+        <f t="shared" si="6"/>
+        <v>335</v>
+      </c>
+      <c r="E50" s="49">
+        <f t="shared" si="7"/>
+        <v>1040</v>
+      </c>
+      <c r="F50" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G50" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H50" s="41">
+        <v>0</v>
+      </c>
+      <c r="I50" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="J50" s="49"/>
+    </row>
+    <row r="51" spans="1:10" ht="15.75">
+      <c r="A51" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="49">
+        <v>150</v>
+      </c>
+      <c r="C51" s="49">
+        <v>193</v>
+      </c>
+      <c r="D51" s="49">
+        <f t="shared" si="6"/>
+        <v>150</v>
+      </c>
+      <c r="E51" s="49">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="F51" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G51" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H51" s="41">
+        <v>0</v>
+      </c>
+      <c r="I51" s="69" t="s">
+        <v>102</v>
+      </c>
+      <c r="J51" s="71" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75">
+      <c r="A52" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="49">
+        <v>250</v>
+      </c>
+      <c r="C52" s="49">
+        <v>193</v>
+      </c>
+      <c r="D52" s="49">
+        <f t="shared" si="6"/>
+        <v>250</v>
+      </c>
+      <c r="E52" s="49">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="F52" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G52" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H52" s="41">
+        <v>0</v>
+      </c>
+      <c r="I52" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="J52" s="55"/>
+    </row>
+    <row r="53" spans="1:10" ht="15.75">
+      <c r="A53" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" s="49">
+        <v>350</v>
+      </c>
+      <c r="C53" s="49">
+        <v>193</v>
+      </c>
+      <c r="D53" s="49">
+        <f t="shared" si="6"/>
+        <v>350</v>
+      </c>
+      <c r="E53" s="49">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="F53" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G53" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H53" s="41">
+        <v>0</v>
+      </c>
+      <c r="I53" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="J53" s="55"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75">
+      <c r="A54" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="49">
+        <v>450</v>
+      </c>
+      <c r="C54" s="49">
+        <v>193</v>
+      </c>
+      <c r="D54" s="49">
+        <f t="shared" si="6"/>
+        <v>450</v>
+      </c>
+      <c r="E54" s="49">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="F54" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G54" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H54" s="41">
+        <v>0</v>
+      </c>
+      <c r="I54" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="J54" s="55"/>
+    </row>
+    <row r="55" spans="1:10" ht="15.75">
+      <c r="A55" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="49">
+        <v>550</v>
+      </c>
+      <c r="C55" s="49">
+        <v>193</v>
+      </c>
+      <c r="D55" s="49">
+        <f t="shared" si="6"/>
+        <v>550</v>
+      </c>
+      <c r="E55" s="49">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="F55" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G55" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H55" s="41">
+        <v>0</v>
+      </c>
+      <c r="I55" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="J55" s="55"/>
+    </row>
+    <row r="56" spans="1:10" ht="15.75">
+      <c r="A56" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="49">
+        <v>650</v>
+      </c>
+      <c r="C56" s="49">
+        <v>193</v>
+      </c>
+      <c r="D56" s="49">
+        <f t="shared" si="6"/>
+        <v>650</v>
+      </c>
+      <c r="E56" s="49">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="F56" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G56" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H56" s="41">
+        <v>0</v>
+      </c>
+      <c r="I56" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="J56" s="55"/>
+    </row>
+    <row r="57" spans="1:10" ht="15.75">
+      <c r="A57" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="49">
+        <v>750</v>
+      </c>
+      <c r="C57" s="49">
+        <v>193</v>
+      </c>
+      <c r="D57" s="49">
+        <f t="shared" si="6"/>
+        <v>750</v>
+      </c>
+      <c r="E57" s="49">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="F57" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G57" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H57" s="41">
+        <v>0</v>
+      </c>
+      <c r="I57" s="69" t="s">
+        <v>108</v>
+      </c>
+      <c r="J57" s="55"/>
+    </row>
+    <row r="58" spans="1:10" ht="15.75">
+      <c r="A58" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" s="49">
+        <v>850</v>
+      </c>
+      <c r="C58" s="49">
+        <v>193</v>
+      </c>
+      <c r="D58" s="49">
+        <f t="shared" si="6"/>
+        <v>850</v>
+      </c>
+      <c r="E58" s="49">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="F58" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G58" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H58" s="41">
+        <v>0</v>
+      </c>
+      <c r="I58" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="J58" s="55"/>
+    </row>
+    <row r="59" spans="1:10" ht="15.75">
+      <c r="A59" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" s="49">
+        <v>950</v>
+      </c>
+      <c r="C59" s="49">
+        <v>193</v>
+      </c>
+      <c r="D59" s="49">
+        <f t="shared" si="6"/>
+        <v>950</v>
+      </c>
+      <c r="E59" s="49">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="F59" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G59" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H59" s="41">
+        <v>0</v>
+      </c>
+      <c r="I59" s="69" t="s">
+        <v>110</v>
+      </c>
+      <c r="J59" s="56"/>
+    </row>
+    <row r="60" spans="1:10" ht="15.75">
+      <c r="A60" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="B60" s="49">
+        <v>1770</v>
+      </c>
+      <c r="C60" s="49">
+        <v>60</v>
+      </c>
+      <c r="D60" s="49">
+        <f t="shared" si="6"/>
+        <v>1770</v>
+      </c>
+      <c r="E60" s="49">
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+      <c r="F60" s="32">
+        <v>2000</v>
+      </c>
+      <c r="G60" s="23">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="H60" s="41">
+        <v>0</v>
+      </c>
+      <c r="I60" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="J60" s="71" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15.75">
+      <c r="A61" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61" s="49">
+        <v>680</v>
+      </c>
+      <c r="C61" s="49">
+        <v>840</v>
+      </c>
+      <c r="D61" s="49">
+        <f>B61</f>
+        <v>680</v>
+      </c>
+      <c r="E61" s="49">
+        <f>C61</f>
+        <v>840</v>
+      </c>
+      <c r="F61" s="32">
+        <v>2000</v>
+      </c>
+      <c r="G61" s="23">
+        <f>F61/1000</f>
+        <v>2</v>
+      </c>
+      <c r="H61" s="41">
+        <v>0</v>
+      </c>
+      <c r="I61" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="J61" s="56"/>
+    </row>
+    <row r="62" spans="1:10" ht="15.75">
+      <c r="A62" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="49">
+        <v>1240</v>
+      </c>
+      <c r="C62" s="49">
+        <v>840</v>
+      </c>
+      <c r="D62" s="49">
+        <f>B62</f>
+        <v>1240</v>
+      </c>
+      <c r="E62" s="49">
+        <f>C62</f>
+        <v>840</v>
+      </c>
+      <c r="F62" s="32">
+        <v>30000</v>
+      </c>
+      <c r="G62" s="23">
+        <f>F62/1000</f>
+        <v>30</v>
+      </c>
+      <c r="H62" s="41">
+        <v>0</v>
+      </c>
+      <c r="I62" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="J62" s="49" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75">
+      <c r="A63" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" s="49">
+        <v>250</v>
+      </c>
+      <c r="C63" s="49">
+        <v>1040</v>
+      </c>
+      <c r="D63" s="49">
+        <f>B63</f>
+        <v>250</v>
+      </c>
+      <c r="E63" s="49">
+        <f>C63</f>
+        <v>1040</v>
+      </c>
+      <c r="F63" s="32">
+        <v>2000</v>
+      </c>
+      <c r="G63" s="23">
+        <f>F63/1000</f>
+        <v>2</v>
+      </c>
+      <c r="H63" s="41">
+        <v>0</v>
+      </c>
+      <c r="I63" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="J63" s="49"/>
+    </row>
+    <row r="64" spans="1:10" ht="15.75">
+      <c r="A64" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="49">
+        <v>670</v>
+      </c>
+      <c r="C64" s="49">
+        <v>475</v>
+      </c>
+      <c r="D64" s="49">
+        <f>B64</f>
+        <v>670</v>
+      </c>
+      <c r="E64" s="49">
+        <f>C64</f>
+        <v>475</v>
+      </c>
+      <c r="F64" s="32">
+        <v>2000</v>
+      </c>
+      <c r="G64" s="23">
+        <f>F64/1000</f>
+        <v>2</v>
+      </c>
+      <c r="H64" s="41">
+        <v>0</v>
+      </c>
+      <c r="I64" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="J64" s="49"/>
+    </row>
+    <row r="65" spans="1:10" ht="15.75">
+      <c r="A65" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" s="49">
+        <v>1260</v>
+      </c>
+      <c r="C65" s="49">
+        <v>840</v>
+      </c>
+      <c r="D65" s="49">
+        <f>B65</f>
+        <v>1260</v>
+      </c>
+      <c r="E65" s="49">
+        <f>C65</f>
+        <v>840</v>
+      </c>
+      <c r="F65" s="32">
+        <v>2000</v>
+      </c>
+      <c r="G65" s="23">
+        <f>F65/1000</f>
+        <v>2</v>
+      </c>
+      <c r="H65" s="41">
+        <v>0</v>
+      </c>
+      <c r="I65" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="J65" s="49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15.75">
+      <c r="A66" s="49" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="49">
+        <v>660</v>
+      </c>
+      <c r="C66" s="49">
+        <v>840</v>
+      </c>
+      <c r="D66" s="49">
+        <f>B66</f>
+        <v>660</v>
+      </c>
+      <c r="E66" s="49">
+        <f>C66</f>
+        <v>840</v>
+      </c>
+      <c r="F66" s="32">
+        <v>2000</v>
+      </c>
+      <c r="G66" s="23">
+        <f>F66/1000</f>
+        <v>2</v>
+      </c>
+      <c r="H66" s="41">
+        <v>0</v>
+      </c>
+      <c r="I66" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="J66" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J51:J59"/>
+    <mergeCell ref="J60:J61"/>
     <mergeCell ref="J28:J32"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J45:J47"/>
@@ -2652,22 +3527,21 @@
     <mergeCell ref="J3:J11"/>
     <mergeCell ref="J12:J16"/>
     <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D1ED9B-9769-3147-ACA8-FB53F75343FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" s="2" t="s">
@@ -2680,20 +3554,21 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872E4D3D-9758-5041-A18A-4E758B0B3A33}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" s="3" t="s">
@@ -2706,19 +3581,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3DB0C5-0FFF-4648-9EBB-FF4CEBBD4F50}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
change some delay time
</commit_message>
<xml_diff>
--- a/FGO/FGO.xlsx
+++ b/FGO/FGO.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\auto_js_scripts\FGO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongl2/Desktop/personal/GitHub/auto_js_scripts/FGO/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B117F64D-3056-5340-8DA8-FAA6A841D235}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="465" windowWidth="32745" windowHeight="20535"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="32700" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pexel LUT" sheetId="1" r:id="rId1"/>
     <sheet name="Measured" sheetId="2" r:id="rId2"/>
     <sheet name="Actual" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -529,15 +530,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="00000"/>
+    <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
   <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -545,7 +546,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -579,7 +580,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -711,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -848,28 +849,43 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -899,24 +915,12 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -951,7 +955,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6B4FA6B-D066-4644-8083-E69566C80E15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6B4FA6B-D066-4644-8083-E69566C80E15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1000,7 +1004,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2E186714-FDDD-E74D-B31E-D615057E762A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E186714-FDDD-E74D-B31E-D615057E762A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1325,40 +1329,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A67" sqref="A67:XFD79"/>
+      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="17.625" style="7" customWidth="1"/>
-    <col min="2" max="5" width="10.875" style="7"/>
-    <col min="6" max="6" width="13.875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="7" customWidth="1"/>
+    <col min="2" max="5" width="10.83203125" style="7"/>
+    <col min="6" max="6" width="13.83203125" style="7" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="22" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="48" customWidth="1"/>
-    <col min="9" max="9" width="31.375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.625" style="16" customWidth="1"/>
-    <col min="11" max="16384" width="10.875" style="5"/>
+    <col min="9" max="9" width="31.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="16" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75">
+    <row r="1" spans="1:12">
       <c r="A1" s="8"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="58" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58" t="s">
+      <c r="E1" s="63"/>
+      <c r="F1" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="58"/>
+      <c r="G1" s="63"/>
       <c r="H1" s="39" t="s">
         <v>77</v>
       </c>
@@ -1372,7 +1376,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
+    <row r="2" spans="1:12">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1407,7 +1411,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
+    <row r="3" spans="1:12">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
@@ -1435,14 +1439,14 @@
       <c r="H3" s="41">
         <v>1</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="64" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75">
+    <row r="4" spans="1:12">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -1470,10 +1474,10 @@
       <c r="H4" s="41">
         <v>1</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75">
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
@@ -1501,10 +1505,10 @@
       <c r="H5" s="41">
         <v>1</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75">
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -1532,10 +1536,10 @@
       <c r="H6" s="41">
         <v>1</v>
       </c>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75">
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -1563,10 +1567,10 @@
       <c r="H7" s="41">
         <v>1</v>
       </c>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75">
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
@@ -1594,10 +1598,10 @@
       <c r="H8" s="41">
         <v>1</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75">
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
@@ -1625,10 +1629,10 @@
       <c r="H9" s="41">
         <v>1</v>
       </c>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75">
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1656,10 +1660,10 @@
       <c r="H10" s="41">
         <v>1</v>
       </c>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75">
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
@@ -1687,10 +1691,10 @@
       <c r="H11" s="41">
         <v>1</v>
       </c>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75">
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
@@ -1718,14 +1722,14 @@
       <c r="H12" s="42">
         <v>0</v>
       </c>
-      <c r="I12" s="61" t="s">
+      <c r="I12" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="61" t="s">
+      <c r="J12" s="66" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
+    <row r="13" spans="1:12">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1753,10 +1757,10 @@
       <c r="H13" s="42">
         <v>0</v>
       </c>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75">
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
@@ -1784,10 +1788,10 @@
       <c r="H14" s="42">
         <v>0</v>
       </c>
-      <c r="I14" s="62"/>
-      <c r="J14" s="62"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75">
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="10" t="s">
         <v>20</v>
       </c>
@@ -1815,10 +1819,10 @@
       <c r="H15" s="42">
         <v>0</v>
       </c>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75">
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="10" t="s">
         <v>21</v>
       </c>
@@ -1846,10 +1850,10 @@
       <c r="H16" s="42">
         <v>0</v>
       </c>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75">
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="11" t="s">
         <v>22</v>
       </c>
@@ -1877,14 +1881,14 @@
       <c r="H17" s="43">
         <v>0</v>
       </c>
-      <c r="I17" s="63" t="s">
+      <c r="I17" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="63" t="s">
+      <c r="J17" s="68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75">
+    <row r="18" spans="1:10">
       <c r="A18" s="11" t="s">
         <v>23</v>
       </c>
@@ -1912,10 +1916,10 @@
       <c r="H18" s="43">
         <v>0</v>
       </c>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75">
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="11" t="s">
         <v>24</v>
       </c>
@@ -1943,10 +1947,10 @@
       <c r="H19" s="43">
         <v>0</v>
       </c>
-      <c r="I19" s="64"/>
-      <c r="J19" s="64"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75">
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
@@ -1981,7 +1985,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75">
+    <row r="21" spans="1:10">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -2016,7 +2020,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75">
+    <row r="22" spans="1:10">
       <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
@@ -2047,7 +2051,7 @@
       <c r="I22" s="53"/>
       <c r="J22" s="53"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75">
+    <row r="23" spans="1:10">
       <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
@@ -2078,7 +2082,7 @@
       <c r="I23" s="53"/>
       <c r="J23" s="53"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75">
+    <row r="24" spans="1:10">
       <c r="A24" s="13" t="s">
         <v>29</v>
       </c>
@@ -2106,14 +2110,14 @@
       <c r="H24" s="45">
         <v>0</v>
       </c>
-      <c r="I24" s="67" t="s">
+      <c r="I24" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="J24" s="67" t="s">
+      <c r="J24" s="54" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75">
+    <row r="25" spans="1:10">
       <c r="A25" s="13" t="s">
         <v>30</v>
       </c>
@@ -2141,10 +2145,10 @@
       <c r="H25" s="45">
         <v>0</v>
       </c>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75">
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
@@ -2172,10 +2176,10 @@
       <c r="H26" s="45">
         <v>0</v>
       </c>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.75">
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="14" t="s">
         <v>34</v>
       </c>
@@ -2210,7 +2214,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75">
+    <row r="28" spans="1:10">
       <c r="A28" s="14" t="s">
         <v>56</v>
       </c>
@@ -2238,14 +2242,14 @@
       <c r="H28" s="46">
         <v>0</v>
       </c>
-      <c r="I28" s="50" t="s">
+      <c r="I28" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="J28" s="50" t="s">
+      <c r="J28" s="59" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75">
+    <row r="29" spans="1:10">
       <c r="A29" s="14" t="s">
         <v>57</v>
       </c>
@@ -2273,10 +2277,10 @@
       <c r="H29" s="46">
         <v>0</v>
       </c>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75">
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="14" t="s">
         <v>58</v>
       </c>
@@ -2304,10 +2308,10 @@
       <c r="H30" s="46">
         <v>0</v>
       </c>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.75">
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="14" t="s">
         <v>59</v>
       </c>
@@ -2335,10 +2339,10 @@
       <c r="H31" s="46">
         <v>0</v>
       </c>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.75">
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="14" t="s">
         <v>60</v>
       </c>
@@ -2366,10 +2370,10 @@
       <c r="H32" s="46">
         <v>0</v>
       </c>
-      <c r="I32" s="51"/>
-      <c r="J32" s="51"/>
-    </row>
-    <row r="33" spans="1:10" ht="15.75">
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="14" t="s">
         <v>61</v>
       </c>
@@ -2404,7 +2408,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75">
+    <row r="34" spans="1:10" ht="20">
       <c r="A34" s="15" t="s">
         <v>41</v>
       </c>
@@ -2439,7 +2443,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75">
+    <row r="35" spans="1:10">
       <c r="A35" s="15" t="s">
         <v>35</v>
       </c>
@@ -2467,14 +2471,14 @@
       <c r="H35" s="47">
         <v>0</v>
       </c>
-      <c r="I35" s="65" t="s">
+      <c r="I35" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="J35" s="65" t="s">
+      <c r="J35" s="70" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75">
+    <row r="36" spans="1:10">
       <c r="A36" s="15" t="s">
         <v>36</v>
       </c>
@@ -2502,10 +2506,10 @@
       <c r="H36" s="47">
         <v>0</v>
       </c>
-      <c r="I36" s="66"/>
-      <c r="J36" s="66"/>
-    </row>
-    <row r="37" spans="1:10" ht="15.75">
+      <c r="I36" s="71"/>
+      <c r="J36" s="71"/>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="15" t="s">
         <v>37</v>
       </c>
@@ -2533,10 +2537,10 @@
       <c r="H37" s="47">
         <v>0</v>
       </c>
-      <c r="I37" s="66"/>
-      <c r="J37" s="66"/>
-    </row>
-    <row r="38" spans="1:10" ht="15.75">
+      <c r="I37" s="71"/>
+      <c r="J37" s="71"/>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="15" t="s">
         <v>38</v>
       </c>
@@ -2564,10 +2568,10 @@
       <c r="H38" s="47">
         <v>0</v>
       </c>
-      <c r="I38" s="66"/>
-      <c r="J38" s="66"/>
-    </row>
-    <row r="39" spans="1:10" ht="15.75">
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="15" t="s">
         <v>39</v>
       </c>
@@ -2595,10 +2599,10 @@
       <c r="H39" s="47">
         <v>0</v>
       </c>
-      <c r="I39" s="66"/>
-      <c r="J39" s="66"/>
-    </row>
-    <row r="40" spans="1:10" ht="15.75">
+      <c r="I39" s="71"/>
+      <c r="J39" s="71"/>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="15" t="s">
         <v>40</v>
       </c>
@@ -2626,10 +2630,10 @@
       <c r="H40" s="47">
         <v>0</v>
       </c>
-      <c r="I40" s="66"/>
-      <c r="J40" s="66"/>
-    </row>
-    <row r="41" spans="1:10" ht="15.75">
+      <c r="I40" s="71"/>
+      <c r="J40" s="71"/>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="18" t="s">
         <v>43</v>
       </c>
@@ -2664,7 +2668,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75">
+    <row r="42" spans="1:10">
       <c r="A42" s="18" t="s">
         <v>53</v>
       </c>
@@ -2699,7 +2703,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75">
+    <row r="43" spans="1:10">
       <c r="A43" s="18" t="s">
         <v>78</v>
       </c>
@@ -2734,7 +2738,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75">
+    <row r="44" spans="1:10">
       <c r="A44" s="19" t="s">
         <v>81</v>
       </c>
@@ -2769,7 +2773,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75">
+    <row r="45" spans="1:10">
       <c r="A45" s="19" t="s">
         <v>82</v>
       </c>
@@ -2787,7 +2791,7 @@
         <f t="shared" si="7"/>
         <v>365</v>
       </c>
-      <c r="F45" s="33">
+      <c r="F45" s="72">
         <v>1500</v>
       </c>
       <c r="G45" s="24">
@@ -2800,11 +2804,11 @@
       <c r="I45" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="J45" s="54" t="s">
+      <c r="J45" s="61" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75">
+    <row r="46" spans="1:10">
       <c r="A46" s="19" t="s">
         <v>85</v>
       </c>
@@ -2822,7 +2826,7 @@
         <f t="shared" si="7"/>
         <v>840</v>
       </c>
-      <c r="F46" s="33">
+      <c r="F46" s="72">
         <v>1500</v>
       </c>
       <c r="G46" s="24">
@@ -2835,9 +2839,9 @@
       <c r="I46" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="J46" s="55"/>
-    </row>
-    <row r="47" spans="1:10" ht="15.75">
+      <c r="J46" s="57"/>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="19" t="s">
         <v>86</v>
       </c>
@@ -2855,7 +2859,7 @@
         <f t="shared" si="7"/>
         <v>840</v>
       </c>
-      <c r="F47" s="33">
+      <c r="F47" s="72">
         <v>3000</v>
       </c>
       <c r="G47" s="24">
@@ -2868,9 +2872,9 @@
       <c r="I47" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="J47" s="56"/>
-    </row>
-    <row r="48" spans="1:10" ht="15.75">
+      <c r="J47" s="58"/>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="49" t="s">
         <v>90</v>
       </c>
@@ -2898,12 +2902,12 @@
       <c r="H48" s="41">
         <v>0</v>
       </c>
-      <c r="I48" s="69" t="s">
+      <c r="I48" s="50" t="s">
         <v>91</v>
       </c>
       <c r="J48" s="49"/>
     </row>
-    <row r="49" spans="1:10" ht="15.75">
+    <row r="49" spans="1:10">
       <c r="A49" s="49" t="s">
         <v>117</v>
       </c>
@@ -2931,13 +2935,13 @@
       <c r="H49" s="41">
         <v>0</v>
       </c>
-      <c r="I49" s="69" t="s">
+      <c r="I49" s="50" t="s">
         <v>118</v>
       </c>
       <c r="J49" s="49"/>
     </row>
-    <row r="50" spans="1:10" ht="15.75">
-      <c r="A50" s="70" t="s">
+    <row r="50" spans="1:10">
+      <c r="A50" s="51" t="s">
         <v>92</v>
       </c>
       <c r="B50" s="49">
@@ -2969,7 +2973,7 @@
       </c>
       <c r="J50" s="49"/>
     </row>
-    <row r="51" spans="1:10" ht="15.75">
+    <row r="51" spans="1:10">
       <c r="A51" s="49" t="s">
         <v>93</v>
       </c>
@@ -2997,14 +3001,14 @@
       <c r="H51" s="41">
         <v>0</v>
       </c>
-      <c r="I51" s="69" t="s">
+      <c r="I51" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="J51" s="71" t="s">
+      <c r="J51" s="56" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15.75">
+    <row r="52" spans="1:10">
       <c r="A52" s="49" t="s">
         <v>94</v>
       </c>
@@ -3032,12 +3036,12 @@
       <c r="H52" s="41">
         <v>0</v>
       </c>
-      <c r="I52" s="69" t="s">
+      <c r="I52" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="J52" s="55"/>
-    </row>
-    <row r="53" spans="1:10" ht="15.75">
+      <c r="J52" s="57"/>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="49" t="s">
         <v>95</v>
       </c>
@@ -3065,12 +3069,12 @@
       <c r="H53" s="41">
         <v>0</v>
       </c>
-      <c r="I53" s="69" t="s">
+      <c r="I53" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="J53" s="55"/>
-    </row>
-    <row r="54" spans="1:10" ht="15.75">
+      <c r="J53" s="57"/>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="49" t="s">
         <v>96</v>
       </c>
@@ -3098,12 +3102,12 @@
       <c r="H54" s="41">
         <v>0</v>
       </c>
-      <c r="I54" s="69" t="s">
+      <c r="I54" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="J54" s="55"/>
-    </row>
-    <row r="55" spans="1:10" ht="15.75">
+      <c r="J54" s="57"/>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="49" t="s">
         <v>97</v>
       </c>
@@ -3131,12 +3135,12 @@
       <c r="H55" s="41">
         <v>0</v>
       </c>
-      <c r="I55" s="69" t="s">
+      <c r="I55" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="J55" s="55"/>
-    </row>
-    <row r="56" spans="1:10" ht="15.75">
+      <c r="J55" s="57"/>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="49" t="s">
         <v>98</v>
       </c>
@@ -3164,12 +3168,12 @@
       <c r="H56" s="41">
         <v>0</v>
       </c>
-      <c r="I56" s="69" t="s">
+      <c r="I56" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="J56" s="55"/>
-    </row>
-    <row r="57" spans="1:10" ht="15.75">
+      <c r="J56" s="57"/>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="49" t="s">
         <v>99</v>
       </c>
@@ -3197,12 +3201,12 @@
       <c r="H57" s="41">
         <v>0</v>
       </c>
-      <c r="I57" s="69" t="s">
+      <c r="I57" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="J57" s="55"/>
-    </row>
-    <row r="58" spans="1:10" ht="15.75">
+      <c r="J57" s="57"/>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="49" t="s">
         <v>100</v>
       </c>
@@ -3230,12 +3234,12 @@
       <c r="H58" s="41">
         <v>0</v>
       </c>
-      <c r="I58" s="69" t="s">
+      <c r="I58" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="J58" s="55"/>
-    </row>
-    <row r="59" spans="1:10" ht="15.75">
+      <c r="J58" s="57"/>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="49" t="s">
         <v>101</v>
       </c>
@@ -3263,12 +3267,12 @@
       <c r="H59" s="41">
         <v>0</v>
       </c>
-      <c r="I59" s="69" t="s">
+      <c r="I59" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="J59" s="56"/>
-    </row>
-    <row r="60" spans="1:10" ht="15.75">
+      <c r="J59" s="58"/>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="49" t="s">
         <v>115</v>
       </c>
@@ -3296,14 +3300,14 @@
       <c r="H60" s="41">
         <v>0</v>
       </c>
-      <c r="I60" s="69" t="s">
+      <c r="I60" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="J60" s="71" t="s">
+      <c r="J60" s="56" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.75">
+    <row r="61" spans="1:10">
       <c r="A61" s="49" t="s">
         <v>114</v>
       </c>
@@ -3314,29 +3318,29 @@
         <v>840</v>
       </c>
       <c r="D61" s="49">
-        <f>B61</f>
+        <f t="shared" ref="D61:E66" si="13">B61</f>
         <v>680</v>
       </c>
       <c r="E61" s="49">
-        <f>C61</f>
+        <f t="shared" si="13"/>
         <v>840</v>
       </c>
       <c r="F61" s="32">
         <v>2000</v>
       </c>
       <c r="G61" s="23">
-        <f>F61/1000</f>
+        <f t="shared" ref="G61:G66" si="14">F61/1000</f>
         <v>2</v>
       </c>
       <c r="H61" s="41">
         <v>0</v>
       </c>
-      <c r="I61" s="69" t="s">
+      <c r="I61" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="J61" s="56"/>
-    </row>
-    <row r="62" spans="1:10" ht="15.75">
+      <c r="J61" s="58"/>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="49" t="s">
         <v>113</v>
       </c>
@@ -3347,31 +3351,31 @@
         <v>840</v>
       </c>
       <c r="D62" s="49">
-        <f>B62</f>
+        <f t="shared" si="13"/>
         <v>1240</v>
       </c>
       <c r="E62" s="49">
-        <f>C62</f>
+        <f t="shared" si="13"/>
         <v>840</v>
       </c>
       <c r="F62" s="32">
         <v>30000</v>
       </c>
       <c r="G62" s="23">
-        <f>F62/1000</f>
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="H62" s="41">
         <v>0</v>
       </c>
-      <c r="I62" s="69" t="s">
+      <c r="I62" s="50" t="s">
         <v>111</v>
       </c>
       <c r="J62" s="49" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15.75">
+    <row r="63" spans="1:10">
       <c r="A63" s="49" t="s">
         <v>125</v>
       </c>
@@ -3382,29 +3386,29 @@
         <v>1040</v>
       </c>
       <c r="D63" s="49">
-        <f>B63</f>
+        <f t="shared" si="13"/>
         <v>250</v>
       </c>
       <c r="E63" s="49">
-        <f>C63</f>
+        <f t="shared" si="13"/>
         <v>1040</v>
       </c>
       <c r="F63" s="32">
         <v>2000</v>
       </c>
       <c r="G63" s="23">
-        <f>F63/1000</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="H63" s="41">
         <v>0</v>
       </c>
-      <c r="I63" s="69" t="s">
+      <c r="I63" s="50" t="s">
         <v>123</v>
       </c>
       <c r="J63" s="49"/>
     </row>
-    <row r="64" spans="1:10" ht="15.75">
+    <row r="64" spans="1:10">
       <c r="A64" s="49" t="s">
         <v>124</v>
       </c>
@@ -3415,29 +3419,29 @@
         <v>475</v>
       </c>
       <c r="D64" s="49">
-        <f>B64</f>
+        <f t="shared" si="13"/>
         <v>670</v>
       </c>
       <c r="E64" s="49">
-        <f>C64</f>
+        <f t="shared" si="13"/>
         <v>475</v>
       </c>
       <c r="F64" s="32">
         <v>2000</v>
       </c>
       <c r="G64" s="23">
-        <f>F64/1000</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="H64" s="41">
         <v>0</v>
       </c>
-      <c r="I64" s="69" t="s">
+      <c r="I64" s="50" t="s">
         <v>128</v>
       </c>
       <c r="J64" s="49"/>
     </row>
-    <row r="65" spans="1:10" ht="15.75">
+    <row r="65" spans="1:10">
       <c r="A65" s="49" t="s">
         <v>126</v>
       </c>
@@ -3448,31 +3452,31 @@
         <v>840</v>
       </c>
       <c r="D65" s="49">
-        <f>B65</f>
+        <f t="shared" si="13"/>
         <v>1260</v>
       </c>
       <c r="E65" s="49">
-        <f>C65</f>
+        <f t="shared" si="13"/>
         <v>840</v>
       </c>
       <c r="F65" s="32">
         <v>2000</v>
       </c>
       <c r="G65" s="23">
-        <f>F65/1000</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="H65" s="41">
         <v>0</v>
       </c>
-      <c r="I65" s="69" t="s">
+      <c r="I65" s="50" t="s">
         <v>129</v>
       </c>
       <c r="J65" s="49" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15.75">
+    <row r="66" spans="1:10">
       <c r="A66" s="49" t="s">
         <v>127</v>
       </c>
@@ -3483,35 +3487,30 @@
         <v>840</v>
       </c>
       <c r="D66" s="49">
-        <f>B66</f>
+        <f t="shared" si="13"/>
         <v>660</v>
       </c>
       <c r="E66" s="49">
-        <f>C66</f>
+        <f t="shared" si="13"/>
         <v>840</v>
       </c>
       <c r="F66" s="32">
         <v>2000</v>
       </c>
       <c r="G66" s="23">
-        <f>F66/1000</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="H66" s="41">
         <v>0</v>
       </c>
-      <c r="I66" s="69" t="s">
+      <c r="I66" s="50" t="s">
         <v>130</v>
       </c>
       <c r="J66" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="J51:J59"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="J28:J32"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J45:J47"/>
     <mergeCell ref="B1:C1"/>
@@ -3527,6 +3526,11 @@
     <mergeCell ref="J3:J11"/>
     <mergeCell ref="J12:J16"/>
     <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J51:J59"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="J28:J32"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3534,14 +3538,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" s="2" t="s">
@@ -3561,14 +3565,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" s="3" t="s">

</xml_diff>